<commit_message>
fix bug detect table 95% correctly
</commit_message>
<xml_diff>
--- a/test_usgs/excel_output/production_reserve_tables1.xlsx
+++ b/test_usgs/excel_output/production_reserve_tables1.xlsx
@@ -506,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,11 +545,6 @@
           <t>text_4</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>text_5</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -560,21 +555,24 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Fused aluminum</t>
+          <t>Fused aluminum oxide</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Fused aluminum</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>Fused aluminum oxide</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Silicon carbide</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Silicon</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+          <t>Silicon carbide</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -590,20 +588,15 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
@@ -627,15 +620,10 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>40,000</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>40,000</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
         <is>
           <t>40,000</t>
         </is>
@@ -659,15 +647,10 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>60,000</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
         <is>
           <t>—</t>
         </is>
@@ -691,15 +674,10 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>50,000</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
         <is>
           <t>—</t>
         </is>
@@ -723,15 +701,10 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>90,000</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
         <is>
           <t>—</t>
         </is>
@@ -755,15 +728,10 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>50,000</t>
+          <t>40,000</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
-        <is>
-          <t>40,000</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
         <is>
           <t>40,000</t>
         </is>
@@ -785,13 +753,12 @@
           <t>800,000</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>450,000</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
-        <is>
-          <t>450,000</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
         <is>
           <t>450,000</t>
         </is>
@@ -813,13 +780,12 @@
           <t>40,000</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>20,000</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr">
-        <is>
-          <t>20,000</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
         <is>
           <t>20,000</t>
         </is>
@@ -841,13 +807,12 @@
           <t>80,000</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>35,000</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
-        <is>
-          <t>35,000</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
         <is>
           <t>35,000</t>
         </is>
@@ -869,13 +834,12 @@
           <t>40,000</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>5,000</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr">
-        <is>
-          <t>5,000</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
         <is>
           <t>5,000</t>
         </is>
@@ -897,13 +861,12 @@
           <t>15,000</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>60,000</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
-        <is>
-          <t>60,000</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
         <is>
           <t>60,000</t>
         </is>
@@ -925,13 +888,12 @@
           <t>—</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>45,000</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
-        <is>
-          <t>45,000</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
         <is>
           <t>45,000</t>
         </is>
@@ -953,13 +915,12 @@
           <t>—</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>80,000</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr">
-        <is>
-          <t>80,000</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
         <is>
           <t>80,000</t>
         </is>
@@ -981,13 +942,12 @@
           <t>—</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>30,000</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
-        <is>
-          <t>30,000</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
         <is>
           <t>30,000</t>
         </is>
@@ -1009,13 +969,12 @@
           <t>80,000</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>200,000</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
-        <is>
-          <t>200,000</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
         <is>
           <t>200,000</t>
         </is>
@@ -1037,13 +996,12 @@
           <t>1,300,000</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1,000,000</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
-        <is>
-          <t>1,000,000</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
         <is>
           <t>1,000,000</t>
         </is>
@@ -1112,7 +1070,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -1367,7 +1329,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -2397,10 +2363,14 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Reserves</t>
@@ -2416,7 +2386,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2023e</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -2788,7 +2758,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -3134,11 +3108,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -3382,7 +3364,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -3637,7 +3623,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -3972,11 +3962,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -4201,11 +4199,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -4548,7 +4554,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5028,7 +5038,11 @@
           <t>Plant production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -5555,7 +5569,11 @@
           <t>Production, all forms</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -6008,7 +6026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6052,11 +6070,6 @@
           <t>text_5</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>text_6</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6067,245 +6080,245 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Alumina</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Bauxite production</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Bauxite production</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Bauxite</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>e920</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>780</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>W</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2023e</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>20,000</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="D4" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>e920</t>
+          <t>19,500</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>19,000</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>102,000</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>20,000</t>
+          <t>98,000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3,500,000</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>19,500</t>
+          <t>10,000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>19,000</t>
+          <t>10,000</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>102,000</t>
+          <t>e30,000</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>98,000</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>3,500,000</t>
+          <t>31,000</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2,700,000</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="D6" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10,000</t>
+          <t>1,360</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10,000</t>
+          <t>1,600</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>e30,000</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>31,000</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2,700,000</t>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="D7" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>China</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1,360</t>
+          <t>81,900</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1,600</t>
+          <t>82,000</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>90,000</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>93,000</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>710,000</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="D8" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>81,900</t>
+          <t>e1,000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>82,000</t>
+          <t>720</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>90,000</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>93,000</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>710,000</t>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>e1,000</t>
+          <t>861</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>720</t>
+          <t>860</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>1,200</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
+          <t>1,200</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>—</t>
         </is>
@@ -6314,337 +6327,327 @@
     <row r="10">
       <c r="D10" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Guinea</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>861</t>
+          <t>340</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>860</t>
+          <t>330</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1,200</t>
+          <t>100,000</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1,200</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>97,000</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>7,400,000</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="D11" t="inlineStr">
         <is>
-          <t>Guinea</t>
+          <t>India</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>7,500</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>7,300</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>100,000</t>
+          <t>24,000</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>97,000</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>7,400,000</t>
+          <t>23,000</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>650,000</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>7,500</t>
+          <t>1,200</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>7,300</t>
+          <t>1,200</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>24,000</t>
+          <t>e21,000</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>23,000</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>650,000</t>
+          <t>20,000</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1,000,000</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="D13" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>1,630</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>1,200</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>1,200</t>
-        </is>
-      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>e21,000</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>20,000</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>1,000,000</t>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1,630</t>
+          <t>634</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1,200</t>
+          <t>1,500</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>4,370</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>6,000</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2,000,000</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>634</t>
+          <t>1,340</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>1,500</t>
+          <t>1,300</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>4,370</t>
+          <t>4,400</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>6,000</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>2,000,000</t>
+          <t>4,300</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>160,000</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="D16" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1,340</t>
+          <t>3,080</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>1,300</t>
+          <t>2,400</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>4,400</t>
+          <t>5,780</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>4,300</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>160,000</t>
+          <t>5,800</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>480,000</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3,080</t>
+          <t>1,900</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2,400</t>
+          <t>1,800</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>5,780</t>
+          <t>4,800</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>5,800</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>480,000</t>
+          <t>4,600</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>180,000</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1,900</t>
+          <t>1,340</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1,800</t>
+          <t>640</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>4,800</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>4,600</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>180,000</t>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1,340</t>
+          <t>300</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>640</t>
+          <t>290</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>2,800</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>2,000</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>63,000</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -6654,54 +6657,52 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>—</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2,800</t>
+          <t>—</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2,000</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>63,000</t>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>2,430</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>2,300</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>—</t>
         </is>
@@ -6710,134 +6711,98 @@
     <row r="22">
       <c r="D22" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2,430</t>
+          <t>1,430</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2,300</t>
+          <t>1,400</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>3,900</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>3,700</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>5,800,000</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Other countries</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1,430</t>
+          <t>1,200</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1,400</t>
+          <t>880</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>3,900</t>
+          <t>5,900</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>3,700</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>5,800,000</t>
+          <t>5,600</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>5,100,000</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="D24" t="inlineStr">
         <is>
-          <t>Other countries</t>
+          <t>World total (rounded)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1,200</t>
+          <t>140,000</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>880</t>
+          <t>140,000</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>5,900</t>
+          <t>400,000</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>5,600</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>5,100,000</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>World total (rounded)</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>140,000</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>140,000</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
           <t>400,000</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>400,000</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>30,000,000</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6902,7 +6867,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -7413,11 +7382,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -7848,7 +7825,11 @@
           <t>Mine production8</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -8095,11 +8076,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -8654,11 +8643,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -8897,7 +8894,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -9284,7 +9285,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -9597,11 +9602,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Refinery</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Refinery production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Refinery production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -9857,12 +9870,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Zirconium</t>
+          <t>Zirconium reserves</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Zirconium</t>
+          <t>Zirconium reserves</t>
         </is>
       </c>
     </row>
@@ -10314,7 +10327,11 @@
           <t>Production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -11040,11 +11057,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Production—All</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Production—All forms</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Production—All forms</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -11339,7 +11364,11 @@
           <t>Production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -11643,7 +11672,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -17072,7 +17105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17116,11 +17149,6 @@
           <t>text_5</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>text_6</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -17147,10 +17175,9 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>PGM</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+          <t>PGM reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -17180,7 +17207,6 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="D4" t="inlineStr"/>
@@ -17205,7 +17231,6 @@
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="D5" t="inlineStr">
@@ -17233,8 +17258,7 @@
           <t>2,900</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>820,000</t>
         </is>
@@ -17266,8 +17290,7 @@
           <t>5,500</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>310,000</t>
         </is>
@@ -17299,8 +17322,7 @@
           <t>23,000</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>5,500,000</t>
         </is>
@@ -17332,8 +17354,7 @@
           <t>120,000</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>63,000,000</t>
         </is>
@@ -17365,8 +17386,7 @@
           <t>19,000</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>1,200,000</t>
         </is>
@@ -17398,8 +17418,7 @@
           <t>4,600</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
@@ -17431,8 +17450,7 @@
           <t>180,000</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>71,000,000</t>
         </is>
@@ -17526,11 +17544,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Refinery</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Refinery production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Refinery production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -17927,11 +17953,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -18213,8 +18247,16 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -18680,7 +18722,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -19130,16 +19176,24 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Cement</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>Cement production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Cement production</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Clinker</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>Clinker capacity</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Clinker capacity</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -20719,11 +20773,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -21177,16 +21239,24 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sponge</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>Sponge production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Sponge production</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Capacity,</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>Capacity, 2023</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Capacity, 2023</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
@@ -21198,7 +21268,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -22389,8 +22463,16 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -23249,11 +23331,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -23566,7 +23656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23600,37 +23690,22 @@
           <t>text_3</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>text_4</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>text_5</t>
-        </is>
-      </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>text_6</t>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>text_1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>text_2</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>text_1</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>text_2</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>text_3</t>
         </is>
@@ -23642,127 +23717,110 @@
           <t>(Data in thousand metric tons, chromium content, unless otherwise specified)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>FY 2023</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>FY 2023</t>
+          <t>Mine production1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>FY 2023</t>
+          <t>Mine production1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>FY 2023</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>FY 2024</t>
+          <t>Reserves1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>FY 2024</t>
-        </is>
-      </c>
+          <t>Mine production1</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Mine production1</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+          <t>Reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Potential acquisitions</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Potential disposals</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Potential disposals</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Potential disposals</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Material</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Potential acquisitions</t>
+          <t>(shipping grade)1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Potential disposals</t>
-        </is>
-      </c>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
           <t>(shipping grade)1</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Ferrochromium:</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>630</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
         <is>
           <t>630</t>
         </is>
@@ -23771,55 +23829,40 @@
     <row r="5">
       <c r="D5" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>321.8</t>
+          <t>2,000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>321.8</t>
+          <t>2,000</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>321.8</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>High carbon</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>8,300</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>321.8</t>
+          <t>2,000</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2,000</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Finland</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
-        <is>
-          <t>2,000</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Finland</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2,000</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
         <is>
           <t>8,300</t>
         </is>
@@ -23828,55 +23871,40 @@
     <row r="6">
       <c r="D6" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>Indiae</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>4,000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>4,200</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Low carbon</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>79,000</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>4,000</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>4,200</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Indiae</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
-        <is>
-          <t>4,000</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Indiae</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>4,200</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
         <is>
           <t>79,000</t>
         </is>
@@ -23885,55 +23913,40 @@
     <row r="7">
       <c r="D7" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.454</t>
+          <t>6,000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.454</t>
+          <t>6,000</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.454</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Chromium metal</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>230,000</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.454</t>
+          <t>6,000</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>6,000</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
-        <is>
-          <t>6,000</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Kazakhstan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>6,000</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
         <is>
           <t>230,000</t>
         </is>
@@ -23942,43 +23955,40 @@
     <row r="8">
       <c r="D8" t="inlineStr">
         <is>
-          <t>South Africa was the leading chromite ore producer. Global chromite ore mine</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>South Africa was the leading chromite ore producer. Global chromite ore mine</t>
+          <t>19,100</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>South Africa was the leading chromite ore producer. Global chromite ore mine</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>South Africa was the leading chromite ore producer. Global chromite ore mine</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+          <t>200,000</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>19,100</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>18,000</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr">
-        <is>
-          <t>19,100</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>18,000</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
         <is>
           <t>200,000</t>
         </is>
@@ -23987,43 +23997,40 @@
     <row r="9">
       <c r="D9" t="inlineStr">
         <is>
-          <t>Events, Trends, and Issues:</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Events, Trends, and Issues:</t>
+          <t>5,410</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Events, Trends, and Issues:</t>
+          <t>6,000</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Events, Trends, and Issues:</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+          <t>27,000</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>5,410</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>6,000</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Turkey</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr">
-        <is>
-          <t>5,410</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>6,000</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
         <is>
           <t>27,000</t>
         </is>
@@ -24032,43 +24039,40 @@
     <row r="10">
       <c r="D10" t="inlineStr">
         <is>
-          <t>production was estimated to have decreased slightly in 2023 compared with production in 2022. Production in South</t>
+          <t>Other countries</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>production was estimated to have decreased slightly in 2023 compared with production in 2022. Production in South</t>
+          <t>5,380</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>production was estimated to have decreased slightly in 2023 compared with production in 2022. Production in South</t>
+          <t>5,200</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>production was estimated to have decreased slightly in 2023 compared with production in 2022. Production in South</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>5,380</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>5,200</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Other countries</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr">
-        <is>
-          <t>5,380</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Other countries</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>5,200</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
@@ -24077,643 +24081,426 @@
     <row r="11">
       <c r="D11" t="inlineStr">
         <is>
-          <t>Africa, the world’s leading producer of chromite, decreased by an estimated 6% compared with production in 2022</t>
+          <t>World total (rounded)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Africa, the world’s leading producer of chromite, decreased by an estimated 6% compared with production in 2022</t>
+          <t>41,900</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Africa, the world’s leading producer of chromite, decreased by an estimated 6% compared with production in 2022</t>
+          <t>41,000</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Africa, the world’s leading producer of chromite, decreased by an estimated 6% compared with production in 2022</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+          <t>560,000</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>41,900</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>41,000</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>World total (rounded)</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>41,900</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>World total (rounded)</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>41,000</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
           <t>560,000</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>owing to disruptions to the supply of electricity and problems with transportation of ore via rail. China was the leading</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>owing to disruptions to the supply of electricity and problems with transportation of ore via rail. China was the leading</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>owing to disruptions to the supply of electricity and problems with transportation of ore via rail. China was the leading</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>owing to disruptions to the supply of electricity and problems with transportation of ore via rail. China was the leading</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>World resources are greater than 12 billion tons of shipping-grade chromite, sufficient to meet</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>World resources are greater than 12 billion tons of shipping-grade chromite, sufficient to meet</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>World Resources:1</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>ferrochromium- and stainless-steel-producing country and the leading chromium-consuming country.</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>ferrochromium- and stainless-steel-producing country and the leading chromium-consuming country.</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>ferrochromium- and stainless-steel-producing country and the leading chromium-consuming country.</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>ferrochromium- and stainless-steel-producing country and the leading chromium-consuming country.</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="M13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>conceivable demand for centuries. World chromium resources are heavily geographically concentrated (95%) in</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>conceivable demand for centuries. World chromium resources are heavily geographically concentrated (95%) in</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Reserves for India and Turkey were revised based on Government reports.</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Reserves for India and Turkey were revised based on Government reports.</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Reserves for India and Turkey were revised based on Government reports.</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Reserves for India and Turkey were revised based on Government reports.</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Kazakhstan and southern Africa; United States chromium resources are mostly in the Stillwater Complex in Montana.</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Kazakhstan and southern Africa; United States chromium resources are mostly in the Stillwater Complex in Montana.</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>World Mine Production and Reserves:</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>World Mine Production and Reserves:</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>World Mine Production and Reserves:</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>World Mine Production and Reserves:</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Chromium has no substitute in stainless steel, the leading end use, or in superalloys, the major strategic</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Chromium has no substitute in stainless steel, the leading end use, or in superalloys, the major strategic</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Mine production1</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Reserves1</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Reserves1</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Reserves1</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="M16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Substitutes:</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Substitutes:</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>(shipping grade)1</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>(shipping grade)1</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="M17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>end use. Chromium-containing scrap can substitute for ferrochromium in some metallurgical uses.</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>end use. Chromium-containing scrap can substitute for ferrochromium in some metallurgical uses.</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>630</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="M18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>Estimated. NA Not available. — Zero.</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Estimated. NA Not available. — Zero.</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Finland</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2,000</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2,000</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>8,300</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>Secondary production is based on reported receipts of all types of stainless-steel scrap.</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Secondary production is based on reported receipts of all types of stainless-steel scrap.</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Indiae</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>4,000</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>4,200</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>79,000</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="M20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>Includes chromium chemicals, chromium metal, chromite ores, ferrochromium, ferrosilicon chromium, and stainless-steel products and scrap.</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Includes chromium chemicals, chromium metal, chromite ores, ferrochromium, ferrosilicon chromium, and stainless-steel products and scrap.</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Kazakhstan</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>6,000</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>6,000</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>230,000</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="M21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>Defined as change in total inventory from prior yearend inventory. Beginning in 2023, Government stock changes no longer available.</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Defined as change in total inventory from prior yearend inventory. Beginning in 2023, Government stock changes no longer available.</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>South Africa</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>19,100</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>18,000</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>200,000</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="M22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>Defined for 2019–22 as production (from mines and secondary) + imports – exports ± adjustments for Government and industry stock changes.</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Defined for 2019–22 as production (from mines and secondary) + imports – exports ± adjustments for Government and industry stock changes.</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>5,410</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>6,000</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>27,000</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="M23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>Beginning in 2023, Government stock changes no longer included.</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Beginning in 2023, Government stock changes no longer included.</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Other countries</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>5,380</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>5,200</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="M24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>Source: CRU Group.</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Source: CRU Group.</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>World total (rounded)</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>41,900</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>41,000</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>560,000</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="M25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>Excludes ferrosilicon chromium.</t>
         </is>
       </c>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Excludes ferrosilicon chromium.</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="M26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>Defined for 2019–22 as imports – exports ± adjustments for Government and industry stock changes. Beginning in 2023, Government stock</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Defined for 2019–22 as imports – exports ± adjustments for Government and industry stock changes. Beginning in 2023, Government stock</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="M27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>changes no longer included.</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>changes no longer included.</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="M28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>Includes chromium metal scrap and stainless-steel scrap.</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Includes chromium metal scrap and stainless-steel scrap.</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="M29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>Includes chromium metal, ferrochromium, and stainless steel.</t>
         </is>
       </c>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Includes chromium metal, ferrochromium, and stainless steel.</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="M30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>0Includes Hong Kong.</t>
         </is>
       </c>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>0Includes Hong Kong.</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="M31" t="inlineStr">
+      <c r="J31" t="inlineStr">
         <is>
           <t>1See Appendix B for definitions.</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>1See Appendix B for definitions.</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="M32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>2Units are thousand metric tons, gross weight.</t>
         </is>
       </c>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2Units are thousand metric tons, gross weight.</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="M33" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>3High-carbon and low-carbon ferrochromium, combined.</t>
         </is>
       </c>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>3High-carbon and low-carbon ferrochromium, combined.</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="M34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>4Units are thousand metric tons, gross weight, of marketable chromite ore.</t>
         </is>
       </c>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>4Units are thousand metric tons, gross weight, of marketable chromite ore.</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="M35" t="inlineStr">
+      <c r="J35" t="inlineStr">
         <is>
           <t>5See Appendix C for resource and reserve definitions and information concerning data sources.</t>
         </is>
       </c>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>5See Appendix C for resource and reserve definitions and information concerning data sources.</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="M36" t="inlineStr">
+      <c r="J36" t="inlineStr">
         <is>
           <t>6Units are thousand metric tons of shipping-grade chromite ore, which is deposit quantity and grade normalized to 45% CrO,except for the</t>
         </is>
       </c>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>6Units are thousand metric tons of shipping-grade chromite ore, which is deposit quantity and grade normalized to 45% CrO,except for the</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="M37" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>United States, where grade is normalized to 7%</t>
         </is>
       </c>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>United States, where grade is normalized to 7%</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="M38" t="inlineStr">
+      <c r="J38" t="inlineStr">
         <is>
           <t>CrO, and Finland, where grade is normalized to 26% CrO.</t>
         </is>
       </c>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>CrO, and Finland, where grade is normalized to 26% CrO.</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24770,11 +24557,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -25043,11 +24838,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -25478,7 +25281,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -26689,11 +26496,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -27221,11 +27036,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -27582,11 +27405,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -27973,7 +27804,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -28385,11 +28220,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -28634,7 +28477,11 @@
           <t>Refinery production</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -29299,7 +29146,11 @@
           <t>Production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -30410,11 +30261,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -30996,7 +30855,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -31273,7 +31136,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -31594,7 +31461,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -32450,11 +32321,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -32897,18 +32776,30 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Smelter</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -32924,18 +32815,26 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>W</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Magnesium metal can be derived from</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="D4" t="inlineStr">
@@ -32960,22 +32859,22 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>22</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Magnesium metal can be derived from</t>
+          <t>seawater, natural brines, dolomite,</t>
         </is>
       </c>
     </row>
@@ -33002,22 +32901,22 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>China</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>933</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>830</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>seawater, natural brines, dolomite,</t>
+          <t>serpentine, and other minerals. The</t>
         </is>
       </c>
     </row>
@@ -33044,22 +32943,22 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>933</t>
+          <t>5</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>830</t>
+          <t>5</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>serpentine, and other minerals. The</t>
+          <t>reserves for this metal are sufficient to</t>
         </is>
       </c>
     </row>
@@ -33086,22 +32985,22 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>22</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>reserves for this metal are sufficient to</t>
+          <t>supply current and future requirements.</t>
         </is>
       </c>
     </row>
@@ -33128,24 +33027,20 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>27</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>supply current and future requirements.</t>
-        </is>
-      </c>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="D9" t="inlineStr">
@@ -33170,17 +33065,17 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>21</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>20</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -33208,17 +33103,17 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>14</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
@@ -33246,17 +33141,17 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>—</t>
         </is>
       </c>
       <c r="M11" t="inlineStr"/>
@@ -33284,17 +33179,17 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>World total (rounded)</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1,050</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>940</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -33320,22 +33215,6 @@
           <t>2,300,000</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>World total (rounded)</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>1,050</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>940</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="D14" t="inlineStr">
@@ -33557,11 +33436,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -33926,7 +33813,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -34310,11 +34201,19 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mine</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mine production</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -34745,7 +34644,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>
@@ -35633,7 +35536,11 @@
           <t>Mine production</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Reserves</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr"/>

</xml_diff>